<commit_message>
Este documento fue elaborado por Carolina Arce y por Michael Martinez,con la finalidadde tener las priorizaciones con el objetivo de determinar los sprint del sistema
</commit_message>
<xml_diff>
--- a/Diseño/Priorización.xlsx
+++ b/Diseño/Priorización.xlsx
@@ -498,14 +498,14 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1224,16 +1224,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AW201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A146" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B155" sqref="B155"/>
+    <sheetView tabSelected="1" topLeftCell="A172" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="7.85546875" style="7" customWidth="1"/>
     <col min="2" max="2" width="56.42578125" style="14" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" customWidth="1"/>
-    <col min="4" max="11" width="7.85546875" customWidth="1"/>
+    <col min="3" max="4" width="7.5703125" customWidth="1"/>
+    <col min="5" max="11" width="7.85546875" customWidth="1"/>
     <col min="12" max="14" width="7.42578125" customWidth="1"/>
     <col min="15" max="15" width="7.85546875" customWidth="1"/>
     <col min="16" max="16" width="7.42578125" customWidth="1"/>
@@ -19194,10 +19194,10 @@
       <c r="B104" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="C104" s="26" t="s">
+      <c r="C104" s="25" t="s">
         <v>99</v>
       </c>
-      <c r="D104" s="26"/>
+      <c r="D104" s="25"/>
     </row>
     <row r="105" spans="1:49" ht="15" customHeight="1">
       <c r="A105" s="9" t="s">
@@ -19206,11 +19206,11 @@
       <c r="B105" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="C105" s="25">
+      <c r="C105" s="24">
         <f>+GEOMEAN(C54:AW54)</f>
         <v>8.8258455601063508E-3</v>
       </c>
-      <c r="D105" s="25"/>
+      <c r="D105" s="24"/>
     </row>
     <row r="106" spans="1:49" ht="15" customHeight="1">
       <c r="A106" s="9" t="s">
@@ -19219,11 +19219,11 @@
       <c r="B106" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="C106" s="25">
+      <c r="C106" s="24">
         <f t="shared" ref="C106:C151" si="69">+GEOMEAN(C55:AW55)</f>
         <v>2.5100872154583259E-2</v>
       </c>
-      <c r="D106" s="25"/>
+      <c r="D106" s="24"/>
     </row>
     <row r="107" spans="1:49" ht="15" customHeight="1">
       <c r="A107" s="9" t="s">
@@ -19232,11 +19232,11 @@
       <c r="B107" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="C107" s="25">
+      <c r="C107" s="24">
         <f t="shared" si="69"/>
         <v>1.4780703284271089E-2</v>
       </c>
-      <c r="D107" s="25"/>
+      <c r="D107" s="24"/>
     </row>
     <row r="108" spans="1:49" ht="15" customHeight="1">
       <c r="A108" s="9" t="s">
@@ -19245,11 +19245,11 @@
       <c r="B108" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="C108" s="25">
+      <c r="C108" s="24">
         <f t="shared" si="69"/>
         <v>1.0320618306643006E-2</v>
       </c>
-      <c r="D108" s="25"/>
+      <c r="D108" s="24"/>
     </row>
     <row r="109" spans="1:49" ht="15" customHeight="1">
       <c r="A109" s="9" t="s">
@@ -19258,11 +19258,11 @@
       <c r="B109" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="C109" s="25">
+      <c r="C109" s="24">
         <f t="shared" si="69"/>
         <v>1.8990776188004002E-2</v>
       </c>
-      <c r="D109" s="25"/>
+      <c r="D109" s="24"/>
     </row>
     <row r="110" spans="1:49" ht="15" customHeight="1">
       <c r="A110" s="9" t="s">
@@ -19271,11 +19271,11 @@
       <c r="B110" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="C110" s="25">
+      <c r="C110" s="24">
         <f t="shared" si="69"/>
         <v>2.9855500800090189E-2</v>
       </c>
-      <c r="D110" s="25"/>
+      <c r="D110" s="24"/>
     </row>
     <row r="111" spans="1:49" ht="15" customHeight="1">
       <c r="A111" s="9" t="s">
@@ -19284,11 +19284,11 @@
       <c r="B111" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="C111" s="25">
+      <c r="C111" s="24">
         <f t="shared" si="69"/>
         <v>1.6336909049668336E-2</v>
       </c>
-      <c r="D111" s="25"/>
+      <c r="D111" s="24"/>
     </row>
     <row r="112" spans="1:49" ht="15" customHeight="1">
       <c r="A112" s="9" t="s">
@@ -19297,11 +19297,11 @@
       <c r="B112" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="C112" s="25">
+      <c r="C112" s="24">
         <f t="shared" si="69"/>
         <v>1.9087717539907036E-2</v>
       </c>
-      <c r="D112" s="25"/>
+      <c r="D112" s="24"/>
     </row>
     <row r="113" spans="1:4" ht="15" customHeight="1">
       <c r="A113" s="9" t="s">
@@ -19310,11 +19310,11 @@
       <c r="B113" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="C113" s="25">
+      <c r="C113" s="24">
         <f t="shared" si="69"/>
         <v>3.5331406267766784E-2</v>
       </c>
-      <c r="D113" s="25"/>
+      <c r="D113" s="24"/>
     </row>
     <row r="114" spans="1:4" ht="15" customHeight="1">
       <c r="A114" s="9" t="s">
@@ -19323,11 +19323,11 @@
       <c r="B114" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="C114" s="25">
+      <c r="C114" s="24">
         <f t="shared" si="69"/>
         <v>1.9616474355982672E-2</v>
       </c>
-      <c r="D114" s="25"/>
+      <c r="D114" s="24"/>
     </row>
     <row r="115" spans="1:4" ht="15" customHeight="1">
       <c r="A115" s="9" t="s">
@@ -19336,11 +19336,11 @@
       <c r="B115" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="C115" s="25">
+      <c r="C115" s="24">
         <f t="shared" si="69"/>
         <v>4.0840474157933085E-2</v>
       </c>
-      <c r="D115" s="25"/>
+      <c r="D115" s="24"/>
     </row>
     <row r="116" spans="1:4" ht="15" customHeight="1">
       <c r="A116" s="9" t="s">
@@ -19349,11 +19349,11 @@
       <c r="B116" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="C116" s="25">
+      <c r="C116" s="24">
         <f t="shared" si="69"/>
         <v>2.8760335412970253E-2</v>
       </c>
-      <c r="D116" s="25"/>
+      <c r="D116" s="24"/>
     </row>
     <row r="117" spans="1:4" ht="15" customHeight="1">
       <c r="A117" s="9" t="s">
@@ -19362,11 +19362,11 @@
       <c r="B117" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="C117" s="25">
+      <c r="C117" s="24">
         <f t="shared" si="69"/>
         <v>2.1891192906048188E-2</v>
       </c>
-      <c r="D117" s="25"/>
+      <c r="D117" s="24"/>
     </row>
     <row r="118" spans="1:4" ht="15" customHeight="1">
       <c r="A118" s="9" t="s">
@@ -19375,11 +19375,11 @@
       <c r="B118" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="C118" s="25">
+      <c r="C118" s="24">
         <f t="shared" si="69"/>
         <v>1.6396296844918133E-2</v>
       </c>
-      <c r="D118" s="25"/>
+      <c r="D118" s="24"/>
     </row>
     <row r="119" spans="1:4" ht="15" customHeight="1">
       <c r="A119" s="9" t="s">
@@ -19388,11 +19388,11 @@
       <c r="B119" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="C119" s="25">
+      <c r="C119" s="24">
         <f t="shared" si="69"/>
         <v>8.7167727822560701E-3</v>
       </c>
-      <c r="D119" s="25"/>
+      <c r="D119" s="24"/>
     </row>
     <row r="120" spans="1:4" ht="15" customHeight="1">
       <c r="A120" s="9" t="s">
@@ -19401,11 +19401,11 @@
       <c r="B120" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="C120" s="25">
+      <c r="C120" s="24">
         <f t="shared" si="69"/>
         <v>8.0331151096103871E-3</v>
       </c>
-      <c r="D120" s="25"/>
+      <c r="D120" s="24"/>
     </row>
     <row r="121" spans="1:4" ht="15" customHeight="1">
       <c r="A121" s="9" t="s">
@@ -19414,11 +19414,11 @@
       <c r="B121" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="C121" s="25">
+      <c r="C121" s="24">
         <f t="shared" si="69"/>
         <v>6.8925212799237981E-3</v>
       </c>
-      <c r="D121" s="25"/>
+      <c r="D121" s="24"/>
     </row>
     <row r="122" spans="1:4" ht="15" customHeight="1">
       <c r="A122" s="9" t="s">
@@ -19427,11 +19427,11 @@
       <c r="B122" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="C122" s="25">
+      <c r="C122" s="24">
         <f t="shared" si="69"/>
         <v>1.2505023022148417E-2</v>
       </c>
-      <c r="D122" s="25"/>
+      <c r="D122" s="24"/>
     </row>
     <row r="123" spans="1:4" ht="15" customHeight="1">
       <c r="A123" s="9" t="s">
@@ -19440,11 +19440,11 @@
       <c r="B123" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="C123" s="25">
+      <c r="C123" s="24">
         <f t="shared" si="69"/>
         <v>1.2385917886864392E-2</v>
       </c>
-      <c r="D123" s="25"/>
+      <c r="D123" s="24"/>
     </row>
     <row r="124" spans="1:4" ht="15" customHeight="1">
       <c r="A124" s="9" t="s">
@@ -19453,11 +19453,11 @@
       <c r="B124" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="C124" s="25">
+      <c r="C124" s="24">
         <f t="shared" si="69"/>
         <v>2.0891577646590168E-2</v>
       </c>
-      <c r="D124" s="25"/>
+      <c r="D124" s="24"/>
     </row>
     <row r="125" spans="1:4" ht="15" customHeight="1">
       <c r="A125" s="9" t="s">
@@ -19466,11 +19466,11 @@
       <c r="B125" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="C125" s="25">
+      <c r="C125" s="24">
         <f t="shared" si="69"/>
         <v>1.1034694864224646E-2</v>
       </c>
-      <c r="D125" s="25"/>
+      <c r="D125" s="24"/>
     </row>
     <row r="126" spans="1:4" ht="15" customHeight="1">
       <c r="A126" s="9" t="s">
@@ -19479,11 +19479,11 @@
       <c r="B126" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="C126" s="25">
+      <c r="C126" s="24">
         <f t="shared" si="69"/>
         <v>2.8712606338541356E-2</v>
       </c>
-      <c r="D126" s="25"/>
+      <c r="D126" s="24"/>
     </row>
     <row r="127" spans="1:4" ht="15" customHeight="1">
       <c r="A127" s="9" t="s">
@@ -19492,11 +19492,11 @@
       <c r="B127" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="C127" s="25">
+      <c r="C127" s="24">
         <f t="shared" si="69"/>
         <v>1.0660100476082984E-2</v>
       </c>
-      <c r="D127" s="25"/>
+      <c r="D127" s="24"/>
     </row>
     <row r="128" spans="1:4" ht="15" customHeight="1">
       <c r="A128" s="9" t="s">
@@ -19505,11 +19505,11 @@
       <c r="B128" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="C128" s="25">
+      <c r="C128" s="24">
         <f t="shared" si="69"/>
         <v>1.9653737422132125E-2</v>
       </c>
-      <c r="D128" s="25"/>
+      <c r="D128" s="24"/>
     </row>
     <row r="129" spans="1:4" ht="15" customHeight="1">
       <c r="A129" s="9" t="s">
@@ -19518,11 +19518,11 @@
       <c r="B129" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="C129" s="25">
+      <c r="C129" s="24">
         <f t="shared" si="69"/>
         <v>1.0369692896602788E-2</v>
       </c>
-      <c r="D129" s="25"/>
+      <c r="D129" s="24"/>
     </row>
     <row r="130" spans="1:4" ht="15" customHeight="1">
       <c r="A130" s="9" t="s">
@@ -19531,11 +19531,11 @@
       <c r="B130" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="C130" s="25">
+      <c r="C130" s="24">
         <f t="shared" si="69"/>
         <v>1.0721828059882896E-2</v>
       </c>
-      <c r="D130" s="25"/>
+      <c r="D130" s="24"/>
     </row>
     <row r="131" spans="1:4" ht="15" customHeight="1">
       <c r="A131" s="9" t="s">
@@ -19544,11 +19544,11 @@
       <c r="B131" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="C131" s="25">
+      <c r="C131" s="24">
         <f t="shared" si="69"/>
         <v>8.0760618155907085E-3</v>
       </c>
-      <c r="D131" s="25"/>
+      <c r="D131" s="24"/>
     </row>
     <row r="132" spans="1:4" ht="15" customHeight="1">
       <c r="A132" s="9" t="s">
@@ -19557,11 +19557,11 @@
       <c r="B132" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="C132" s="25">
+      <c r="C132" s="24">
         <f t="shared" si="69"/>
         <v>7.1430946738208368E-3</v>
       </c>
-      <c r="D132" s="25"/>
+      <c r="D132" s="24"/>
     </row>
     <row r="133" spans="1:4" ht="15" customHeight="1">
       <c r="A133" s="9" t="s">
@@ -19570,11 +19570,11 @@
       <c r="B133" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="C133" s="25">
+      <c r="C133" s="24">
         <f t="shared" si="69"/>
         <v>2.5334271224432634E-2</v>
       </c>
-      <c r="D133" s="25"/>
+      <c r="D133" s="24"/>
     </row>
     <row r="134" spans="1:4" ht="15" customHeight="1">
       <c r="A134" s="9" t="s">
@@ -19583,11 +19583,11 @@
       <c r="B134" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="C134" s="25">
+      <c r="C134" s="24">
         <f t="shared" si="69"/>
         <v>2.5637722238189737E-2</v>
       </c>
-      <c r="D134" s="25"/>
+      <c r="D134" s="24"/>
     </row>
     <row r="135" spans="1:4" ht="15" customHeight="1">
       <c r="A135" s="9" t="s">
@@ -19596,11 +19596,11 @@
       <c r="B135" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="C135" s="25">
+      <c r="C135" s="24">
         <f t="shared" si="69"/>
         <v>2.5637722238189737E-2</v>
       </c>
-      <c r="D135" s="25"/>
+      <c r="D135" s="24"/>
     </row>
     <row r="136" spans="1:4" ht="15" customHeight="1">
       <c r="A136" s="9" t="s">
@@ -19609,11 +19609,11 @@
       <c r="B136" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="C136" s="25">
+      <c r="C136" s="24">
         <f t="shared" si="69"/>
         <v>2.185001372809791E-2</v>
       </c>
-      <c r="D136" s="25"/>
+      <c r="D136" s="24"/>
     </row>
     <row r="137" spans="1:4" ht="15" customHeight="1">
       <c r="A137" s="9" t="s">
@@ -19622,11 +19622,11 @@
       <c r="B137" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="C137" s="25">
+      <c r="C137" s="24">
         <f t="shared" si="69"/>
         <v>2.2075590236714453E-2</v>
       </c>
-      <c r="D137" s="25"/>
+      <c r="D137" s="24"/>
     </row>
     <row r="138" spans="1:4" ht="15" customHeight="1">
       <c r="A138" s="9" t="s">
@@ -19635,11 +19635,11 @@
       <c r="B138" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="C138" s="25">
+      <c r="C138" s="24">
         <f t="shared" si="69"/>
         <v>2.1500750578241599E-2</v>
       </c>
-      <c r="D138" s="25"/>
+      <c r="D138" s="24"/>
     </row>
     <row r="139" spans="1:4" ht="15" customHeight="1">
       <c r="A139" s="9" t="s">
@@ -19648,11 +19648,11 @@
       <c r="B139" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="C139" s="25">
+      <c r="C139" s="24">
         <f t="shared" si="69"/>
         <v>1.8202314102537302E-2</v>
       </c>
-      <c r="D139" s="25"/>
+      <c r="D139" s="24"/>
     </row>
     <row r="140" spans="1:4" ht="15" customHeight="1">
       <c r="A140" s="9" t="s">
@@ -19661,11 +19661,11 @@
       <c r="B140" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="C140" s="25">
+      <c r="C140" s="24">
         <f t="shared" si="69"/>
         <v>1.7541352727139237E-2</v>
       </c>
-      <c r="D140" s="25"/>
+      <c r="D140" s="24"/>
     </row>
     <row r="141" spans="1:4" ht="15" customHeight="1">
       <c r="A141" s="9" t="s">
@@ -19674,11 +19674,11 @@
       <c r="B141" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="C141" s="25">
+      <c r="C141" s="24">
         <f t="shared" si="69"/>
         <v>1.7327933421272222E-2</v>
       </c>
-      <c r="D141" s="25"/>
+      <c r="D141" s="24"/>
     </row>
     <row r="142" spans="1:4" ht="15" customHeight="1">
       <c r="A142" s="9" t="s">
@@ -19687,11 +19687,11 @@
       <c r="B142" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="C142" s="25">
+      <c r="C142" s="24">
         <f t="shared" si="69"/>
         <v>1.6638451277915502E-2</v>
       </c>
-      <c r="D142" s="25"/>
+      <c r="D142" s="24"/>
     </row>
     <row r="143" spans="1:4" ht="15" customHeight="1">
       <c r="A143" s="9" t="s">
@@ -19700,11 +19700,11 @@
       <c r="B143" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="C143" s="25">
+      <c r="C143" s="24">
         <f t="shared" si="69"/>
         <v>1.502982025586481E-2</v>
       </c>
-      <c r="D143" s="25"/>
+      <c r="D143" s="24"/>
     </row>
     <row r="144" spans="1:4" ht="15" customHeight="1">
       <c r="A144" s="9" t="s">
@@ -19713,11 +19713,11 @@
       <c r="B144" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="C144" s="25">
+      <c r="C144" s="24">
         <f t="shared" si="69"/>
         <v>1.4809789759280684E-2</v>
       </c>
-      <c r="D144" s="25"/>
+      <c r="D144" s="24"/>
     </row>
     <row r="145" spans="1:4" ht="15" customHeight="1">
       <c r="A145" s="9" t="s">
@@ -19726,11 +19726,11 @@
       <c r="B145" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="C145" s="25">
+      <c r="C145" s="24">
         <f t="shared" si="69"/>
         <v>1.4951114080333476E-2</v>
       </c>
-      <c r="D145" s="25"/>
+      <c r="D145" s="24"/>
     </row>
     <row r="146" spans="1:4" ht="15" customHeight="1">
       <c r="A146" s="9" t="s">
@@ -19739,11 +19739,11 @@
       <c r="B146" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="C146" s="25">
+      <c r="C146" s="24">
         <f t="shared" si="69"/>
         <v>1.4822686819382024E-2</v>
       </c>
-      <c r="D146" s="25"/>
+      <c r="D146" s="24"/>
     </row>
     <row r="147" spans="1:4" ht="15" customHeight="1">
       <c r="A147" s="9" t="s">
@@ -19752,11 +19752,11 @@
       <c r="B147" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="C147" s="25">
+      <c r="C147" s="24">
         <f t="shared" si="69"/>
         <v>1.6088629805829504E-2</v>
       </c>
-      <c r="D147" s="25"/>
+      <c r="D147" s="24"/>
     </row>
     <row r="148" spans="1:4" ht="15" customHeight="1">
       <c r="A148" s="9" t="s">
@@ -19765,11 +19765,11 @@
       <c r="B148" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="C148" s="25">
+      <c r="C148" s="24">
         <f t="shared" si="69"/>
         <v>1.2190472967324402E-2</v>
       </c>
-      <c r="D148" s="25"/>
+      <c r="D148" s="24"/>
     </row>
     <row r="149" spans="1:4" ht="15" customHeight="1">
       <c r="A149" s="9" t="s">
@@ -19778,11 +19778,11 @@
       <c r="B149" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="C149" s="25">
+      <c r="C149" s="24">
         <f t="shared" si="69"/>
         <v>1.5362719426798717E-2</v>
       </c>
-      <c r="D149" s="25"/>
+      <c r="D149" s="24"/>
     </row>
     <row r="150" spans="1:4" ht="15" customHeight="1">
       <c r="A150" s="9" t="s">
@@ -19791,11 +19791,11 @@
       <c r="B150" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="C150" s="25">
+      <c r="C150" s="24">
         <f t="shared" si="69"/>
         <v>3.8143001168874202E-2</v>
       </c>
-      <c r="D150" s="25"/>
+      <c r="D150" s="24"/>
     </row>
     <row r="151" spans="1:4" ht="15" customHeight="1">
       <c r="A151" s="9" t="s">
@@ -19804,19 +19804,19 @@
       <c r="B151" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="C151" s="25">
+      <c r="C151" s="24">
         <f t="shared" si="69"/>
         <v>1.3831102485097054E-2</v>
       </c>
-      <c r="D151" s="25"/>
+      <c r="D151" s="24"/>
     </row>
     <row r="153" spans="1:4" ht="15" customHeight="1">
-      <c r="A153" s="24" t="s">
+      <c r="A153" s="26" t="s">
         <v>100</v>
       </c>
-      <c r="B153" s="24"/>
-      <c r="C153" s="24"/>
-      <c r="D153" s="24"/>
+      <c r="B153" s="26"/>
+      <c r="C153" s="26"/>
+      <c r="D153" s="26"/>
     </row>
     <row r="154" spans="1:4" ht="15" customHeight="1">
       <c r="A154" s="15" t="s">
@@ -20399,12 +20399,37 @@
     <sortCondition descending="1" ref="C155:C201"/>
   </sortState>
   <mergeCells count="49">
-    <mergeCell ref="C109:D109"/>
-    <mergeCell ref="C104:D104"/>
-    <mergeCell ref="C105:D105"/>
-    <mergeCell ref="C106:D106"/>
-    <mergeCell ref="C107:D107"/>
-    <mergeCell ref="C108:D108"/>
+    <mergeCell ref="A153:D153"/>
+    <mergeCell ref="C146:D146"/>
+    <mergeCell ref="C147:D147"/>
+    <mergeCell ref="C148:D148"/>
+    <mergeCell ref="C149:D149"/>
+    <mergeCell ref="C150:D150"/>
+    <mergeCell ref="C151:D151"/>
+    <mergeCell ref="C145:D145"/>
+    <mergeCell ref="C134:D134"/>
+    <mergeCell ref="C135:D135"/>
+    <mergeCell ref="C136:D136"/>
+    <mergeCell ref="C137:D137"/>
+    <mergeCell ref="C138:D138"/>
+    <mergeCell ref="C139:D139"/>
+    <mergeCell ref="C140:D140"/>
+    <mergeCell ref="C141:D141"/>
+    <mergeCell ref="C142:D142"/>
+    <mergeCell ref="C143:D143"/>
+    <mergeCell ref="C144:D144"/>
+    <mergeCell ref="C133:D133"/>
+    <mergeCell ref="C122:D122"/>
+    <mergeCell ref="C123:D123"/>
+    <mergeCell ref="C124:D124"/>
+    <mergeCell ref="C125:D125"/>
+    <mergeCell ref="C126:D126"/>
+    <mergeCell ref="C127:D127"/>
+    <mergeCell ref="C128:D128"/>
+    <mergeCell ref="C129:D129"/>
+    <mergeCell ref="C130:D130"/>
+    <mergeCell ref="C131:D131"/>
+    <mergeCell ref="C132:D132"/>
     <mergeCell ref="C121:D121"/>
     <mergeCell ref="C110:D110"/>
     <mergeCell ref="C111:D111"/>
@@ -20417,37 +20442,12 @@
     <mergeCell ref="C118:D118"/>
     <mergeCell ref="C119:D119"/>
     <mergeCell ref="C120:D120"/>
-    <mergeCell ref="C133:D133"/>
-    <mergeCell ref="C122:D122"/>
-    <mergeCell ref="C123:D123"/>
-    <mergeCell ref="C124:D124"/>
-    <mergeCell ref="C125:D125"/>
-    <mergeCell ref="C126:D126"/>
-    <mergeCell ref="C127:D127"/>
-    <mergeCell ref="C128:D128"/>
-    <mergeCell ref="C129:D129"/>
-    <mergeCell ref="C130:D130"/>
-    <mergeCell ref="C131:D131"/>
-    <mergeCell ref="C132:D132"/>
-    <mergeCell ref="C145:D145"/>
-    <mergeCell ref="C134:D134"/>
-    <mergeCell ref="C135:D135"/>
-    <mergeCell ref="C136:D136"/>
-    <mergeCell ref="C137:D137"/>
-    <mergeCell ref="C138:D138"/>
-    <mergeCell ref="C139:D139"/>
-    <mergeCell ref="C140:D140"/>
-    <mergeCell ref="C141:D141"/>
-    <mergeCell ref="C142:D142"/>
-    <mergeCell ref="C143:D143"/>
-    <mergeCell ref="C144:D144"/>
-    <mergeCell ref="A153:D153"/>
-    <mergeCell ref="C146:D146"/>
-    <mergeCell ref="C147:D147"/>
-    <mergeCell ref="C148:D148"/>
-    <mergeCell ref="C149:D149"/>
-    <mergeCell ref="C150:D150"/>
-    <mergeCell ref="C151:D151"/>
+    <mergeCell ref="C109:D109"/>
+    <mergeCell ref="C104:D104"/>
+    <mergeCell ref="C105:D105"/>
+    <mergeCell ref="C106:D106"/>
+    <mergeCell ref="C107:D107"/>
+    <mergeCell ref="C108:D108"/>
   </mergeCells>
   <pageMargins left="0.11811023622047245" right="0.51181102362204722" top="0.15748031496062992" bottom="0.15748031496062992" header="0.11811023622047245" footer="0.15748031496062992"/>
   <pageSetup scale="50" orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>